<commit_message>
Partial implementation to GEOJson
</commit_message>
<xml_diff>
--- a/Data Modelling Docs/CoinCapDataModel.xlsx
+++ b/Data Modelling Docs/CoinCapDataModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="11175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATA MODEL" sheetId="1" r:id="rId1"/>
@@ -13,26 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DATA MODEL'!$A$2:$G$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DIM TABLES'!$A$1:$D$25</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="173">
   <si>
     <t>RAW_TABLE_NAME</t>
   </si>
@@ -499,7 +487,13 @@
     <t>CURRENCY_ID IS PRIMARY KEY</t>
   </si>
   <si>
+    <t>CURRENCY_TYPE</t>
+  </si>
+  <si>
     <t>DECIMAL(20, 8)</t>
+  </si>
+  <si>
+    <t>SHIFTED TO FACT TABLE</t>
   </si>
   <si>
     <t>EXCHANGE_SR_KEY</t>
@@ -550,14 +544,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,23 +575,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF212121"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -618,16 +626,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -642,16 +642,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -665,7 +681,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -673,16 +703,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -704,28 +727,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -758,13 +760,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,13 +790,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,7 +826,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,19 +874,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -830,13 +892,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,91 +928,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,6 +970,54 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -982,39 +1032,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1025,21 +1042,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1069,152 +1071,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1227,60 +1229,66 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1475,7 +1483,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1484,7 +1492,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1769,14 +1777,14 @@
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88666666666667" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="24.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="22.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="116.888888888889" customWidth="1"/>
-    <col min="4" max="4" width="5.77777777777778" customWidth="1"/>
-    <col min="5" max="5" width="30.5555555555556" customWidth="1"/>
-    <col min="6" max="6" width="43.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="24.22" customWidth="1"/>
+    <col min="2" max="2" width="22.22" customWidth="1"/>
+    <col min="3" max="3" width="116.886666666667" customWidth="1"/>
+    <col min="4" max="4" width="5.78" customWidth="1"/>
+    <col min="5" max="5" width="30.5533333333333" customWidth="1"/>
+    <col min="6" max="6" width="43.22" customWidth="1"/>
     <col min="7" max="7" width="56" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1807,10 +1815,10 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1828,10 +1836,10 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1849,10 +1857,10 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1870,10 +1878,10 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1891,10 +1899,10 @@
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1912,10 +1920,10 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1933,10 +1941,10 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1954,10 +1962,10 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1975,10 +1983,10 @@
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1996,10 +2004,10 @@
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2017,10 +2025,10 @@
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2291,10 +2299,10 @@
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2314,10 +2322,10 @@
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -2337,10 +2345,10 @@
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -2358,10 +2366,10 @@
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2379,10 +2387,10 @@
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -2400,10 +2408,10 @@
       <c r="A30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2421,10 +2429,10 @@
       <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -2442,10 +2450,10 @@
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2463,10 +2471,10 @@
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -2484,10 +2492,10 @@
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2505,10 +2513,10 @@
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2526,10 +2534,10 @@
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="6" t="s">
         <v>81</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2547,10 +2555,10 @@
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2568,10 +2576,10 @@
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2589,10 +2597,10 @@
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2610,10 +2618,10 @@
       <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -2631,10 +2639,10 @@
       <c r="A41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -2654,10 +2662,10 @@
       <c r="A42" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2677,10 +2685,10 @@
       <c r="A43" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="6" t="s">
         <v>74</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2700,10 +2708,10 @@
       <c r="A44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2723,10 +2731,10 @@
       <c r="A45" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="6" t="s">
         <v>81</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2746,10 +2754,10 @@
       <c r="A46" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2769,10 +2777,10 @@
       <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2792,10 +2800,10 @@
       <c r="A48" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2815,10 +2823,10 @@
       <c r="A49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2838,10 +2846,10 @@
       <c r="A50" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2859,10 +2867,10 @@
       <c r="A51" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2880,10 +2888,10 @@
       <c r="A52" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="6" t="s">
         <v>102</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2901,10 +2909,10 @@
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2922,10 +2930,10 @@
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="6" t="s">
         <v>108</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2943,10 +2951,10 @@
       <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2964,10 +2972,10 @@
       <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="6" t="s">
         <v>114</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2985,10 +2993,10 @@
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="6" t="s">
         <v>116</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -3006,10 +3014,10 @@
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="6" t="s">
         <v>118</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -3027,10 +3035,10 @@
       <c r="A59" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="6" t="s">
         <v>121</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -3048,10 +3056,10 @@
       <c r="A60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -3069,10 +3077,10 @@
       <c r="A61" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -3090,10 +3098,10 @@
       <c r="A62" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="6" t="s">
         <v>130</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -3111,10 +3119,10 @@
       <c r="A63" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="6" t="s">
         <v>134</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -3132,10 +3140,10 @@
       <c r="A64" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="6" t="s">
         <v>137</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -3153,10 +3161,10 @@
       <c r="A65" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -3174,10 +3182,10 @@
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="6" t="s">
         <v>143</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -3195,10 +3203,10 @@
       <c r="A67" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="6" t="s">
         <v>146</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -3213,11 +3221,11 @@
       <c r="G67" s="2"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:G67" etc:filterBottomFollowUsedRange="0">
+  <autoFilter ref="A2:G67">
     <filterColumn colId="3">
-      <filters>
-        <filter val="FACT"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="equal" val="FACT"/>
+      </customFilters>
     </filterColumn>
     <extLst/>
   </autoFilter>
@@ -3228,18 +3236,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88666666666667" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="23.1111111111111" customWidth="1"/>
-    <col min="2" max="3" width="32.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="53.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="23.1133333333333" customWidth="1"/>
+    <col min="2" max="3" width="32.8866666666667" customWidth="1"/>
+    <col min="4" max="4" width="53.4466666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3256,7 +3264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" hidden="1" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -3270,7 +3278,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" hidden="1" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -3282,7 +3290,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" hidden="1" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -3294,7 +3302,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" hidden="1" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -3349,7 +3357,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>152</v>
@@ -3357,16 +3365,18 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
@@ -3380,21 +3390,21 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" hidden="1" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" hidden="1" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>70</v>
       </c>
@@ -3406,7 +3416,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" hidden="1" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>70</v>
       </c>
@@ -3418,7 +3428,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" hidden="1" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -3430,7 +3440,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" hidden="1" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>70</v>
       </c>
@@ -3442,7 +3452,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" hidden="1" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -3454,21 +3464,21 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" hidden="1" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
         <v>150</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" hidden="1" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>98</v>
       </c>
@@ -3480,7 +3490,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" hidden="1" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
@@ -3492,7 +3502,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" hidden="1" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>98</v>
       </c>
@@ -3504,7 +3514,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" hidden="1" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>98</v>
       </c>
@@ -3516,7 +3526,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" hidden="1" spans="1:4">
       <c r="A23" s="3" t="s">
         <v>98</v>
       </c>
@@ -3528,24 +3538,24 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" hidden="1" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>150</v>
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" hidden="1" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>150</v>
@@ -3553,6 +3563,14 @@
       <c r="D25" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D25">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="DIM_CURRRENCY_RATE"/>
+      </filters>
+    </filterColumn>
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -3563,15 +3581,15 @@
   <sheetPr/>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="30.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="43.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="30.5533333333333" customWidth="1"/>
+    <col min="2" max="2" width="43.22" customWidth="1"/>
+    <col min="3" max="3" width="14.78" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3590,7 +3608,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>150</v>
@@ -3626,7 +3644,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3637,7 +3655,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3648,7 +3666,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3659,7 +3677,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3670,7 +3688,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3681,7 +3699,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3692,7 +3710,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3703,7 +3721,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3711,7 +3729,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>150</v>
@@ -3722,7 +3740,7 @@
         <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>150</v>
@@ -3733,7 +3751,7 @@
         <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>150</v>
@@ -3744,7 +3762,7 @@
         <v>75</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>150</v>
@@ -3769,7 +3787,7 @@
         <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3780,7 +3798,7 @@
         <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3788,7 +3806,7 @@
         <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>150</v>
@@ -3799,7 +3817,7 @@
         <v>100</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>150</v>
@@ -3810,7 +3828,7 @@
         <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>150</v>
@@ -3835,7 +3853,7 @@
         <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3846,7 +3864,7 @@
         <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3857,7 +3875,7 @@
         <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3868,7 +3886,7 @@
         <v>122</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3887,7 +3905,7 @@
         <v>100</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>150</v>
@@ -3898,7 +3916,7 @@
         <v>131</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>150</v>
@@ -3909,7 +3927,7 @@
         <v>131</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>150</v>
@@ -3923,7 +3941,7 @@
         <v>132</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3934,7 +3952,7 @@
         <v>135</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3945,7 +3963,7 @@
         <v>138</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3956,7 +3974,7 @@
         <v>141</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3967,7 +3985,7 @@
         <v>144</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3975,7 +3993,7 @@
         <v>131</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>150</v>

</xml_diff>